<commit_message>
More data entry with keeler and southwest
</commit_message>
<xml_diff>
--- a/Data/southwest_data.xlsx
+++ b/Data/southwest_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="2500" yWindow="0" windowWidth="25360" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="138">
   <si>
     <t>genus</t>
   </si>
@@ -274,6 +274,165 @@
   </si>
   <si>
     <t>mahaleb</t>
+  </si>
+  <si>
+    <t>emarginata</t>
+  </si>
+  <si>
+    <t>gladulosa</t>
+  </si>
+  <si>
+    <t>minutiflora</t>
+  </si>
+  <si>
+    <t>havardii</t>
+  </si>
+  <si>
+    <t>gracilis</t>
+  </si>
+  <si>
+    <t>murrayana</t>
+  </si>
+  <si>
+    <t>angustifolia</t>
+  </si>
+  <si>
+    <t>reverchonii</t>
+  </si>
+  <si>
+    <t>rivularis</t>
+  </si>
+  <si>
+    <t>persoca</t>
+  </si>
+  <si>
+    <t>Pyrus</t>
+  </si>
+  <si>
+    <t>communis</t>
+  </si>
+  <si>
+    <t>malus</t>
+  </si>
+  <si>
+    <t>Amelanchier</t>
+  </si>
+  <si>
+    <t>denticulata</t>
+  </si>
+  <si>
+    <t>Peraphyllum</t>
+  </si>
+  <si>
+    <t>ramosissimum</t>
+  </si>
+  <si>
+    <t>Rubus</t>
+  </si>
+  <si>
+    <t>sons</t>
+  </si>
+  <si>
+    <t>nefrens</t>
+  </si>
+  <si>
+    <t>serissimus</t>
+  </si>
+  <si>
+    <t>allegheniensis</t>
+  </si>
+  <si>
+    <t>Prosopis</t>
+  </si>
+  <si>
+    <t>pubescens</t>
+  </si>
+  <si>
+    <t>Gymnocladus</t>
+  </si>
+  <si>
+    <t>dioica</t>
+  </si>
+  <si>
+    <t>persistant</t>
+  </si>
+  <si>
+    <t>Cercis</t>
+  </si>
+  <si>
+    <t>canadensis</t>
+  </si>
+  <si>
+    <t>Erythrina</t>
+  </si>
+  <si>
+    <t>flavelliformis</t>
+  </si>
+  <si>
+    <t>Robinia</t>
+  </si>
+  <si>
+    <t>neomexicana</t>
+  </si>
+  <si>
+    <t>Sophora</t>
+  </si>
+  <si>
+    <t>secundiflora</t>
+  </si>
+  <si>
+    <t>Wisteria</t>
+  </si>
+  <si>
+    <t>frutescens</t>
+  </si>
+  <si>
+    <t>Poncirus</t>
+  </si>
+  <si>
+    <t>trifoliata</t>
+  </si>
+  <si>
+    <t>Zanthoxylem</t>
+  </si>
+  <si>
+    <t>americanum</t>
+  </si>
+  <si>
+    <t>dioecious</t>
+  </si>
+  <si>
+    <t>fagara</t>
+  </si>
+  <si>
+    <t>parvum</t>
+  </si>
+  <si>
+    <t>Pistacia</t>
+  </si>
+  <si>
+    <t>texana</t>
+  </si>
+  <si>
+    <t>Rhus</t>
+  </si>
+  <si>
+    <t>aromatica</t>
+  </si>
+  <si>
+    <t>microphylla</t>
+  </si>
+  <si>
+    <t>Ilex</t>
+  </si>
+  <si>
+    <t>decidua</t>
+  </si>
+  <si>
+    <t>early autumn=9</t>
+  </si>
+  <si>
+    <t>montana</t>
   </si>
 </sst>
 </file>
@@ -642,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -914,6 +1073,15 @@
       <c r="H11">
         <v>9.5</v>
       </c>
+      <c r="N11" t="s">
+        <v>111</v>
+      </c>
+      <c r="O11">
+        <v>12</v>
+      </c>
+      <c r="P11" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
@@ -1481,6 +1649,9 @@
       <c r="C35" t="s">
         <v>20</v>
       </c>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
       <c r="E35">
         <v>20</v>
       </c>
@@ -1792,6 +1963,905 @@
       </c>
       <c r="H47">
         <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48">
+        <v>100</v>
+      </c>
+      <c r="F48" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48">
+        <v>4.5</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>68</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H50">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" t="s">
+        <v>68</v>
+      </c>
+      <c r="G52">
+        <v>5.5</v>
+      </c>
+      <c r="H52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" t="s">
+        <v>59</v>
+      </c>
+      <c r="E53">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>68</v>
+      </c>
+      <c r="G54">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55">
+        <v>25</v>
+      </c>
+      <c r="F55" t="s">
+        <v>68</v>
+      </c>
+      <c r="G55">
+        <v>3.5</v>
+      </c>
+      <c r="H55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56" t="s">
+        <v>68</v>
+      </c>
+      <c r="G56">
+        <v>3.5</v>
+      </c>
+      <c r="H56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>59</v>
+      </c>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58">
+        <v>24</v>
+      </c>
+      <c r="F58" t="s">
+        <v>68</v>
+      </c>
+      <c r="G58">
+        <v>4</v>
+      </c>
+      <c r="H58">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59">
+        <v>75</v>
+      </c>
+      <c r="F59" t="s">
+        <v>68</v>
+      </c>
+      <c r="G59">
+        <v>4</v>
+      </c>
+      <c r="H59">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60">
+        <v>50</v>
+      </c>
+      <c r="F60" t="s">
+        <v>68</v>
+      </c>
+      <c r="G60">
+        <v>4.5</v>
+      </c>
+      <c r="H60">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
+      <c r="E61">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>68</v>
+      </c>
+      <c r="G61">
+        <v>2.5</v>
+      </c>
+      <c r="H61">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>59</v>
+      </c>
+      <c r="E62">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62">
+        <v>4.5</v>
+      </c>
+      <c r="H62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63">
+        <v>5.5</v>
+      </c>
+      <c r="H63">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s">
+        <v>59</v>
+      </c>
+      <c r="F64" t="s">
+        <v>68</v>
+      </c>
+      <c r="G64">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" t="s">
+        <v>59</v>
+      </c>
+      <c r="F65" t="s">
+        <v>68</v>
+      </c>
+      <c r="G65">
+        <v>5.5</v>
+      </c>
+      <c r="H65">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>102</v>
+      </c>
+      <c r="B66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E66">
+        <v>4</v>
+      </c>
+      <c r="F66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" t="s">
+        <v>59</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
+        <v>59</v>
+      </c>
+      <c r="E68">
+        <v>30</v>
+      </c>
+      <c r="F68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69">
+        <v>100</v>
+      </c>
+      <c r="F69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G69">
+        <v>5.5</v>
+      </c>
+      <c r="H69">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" t="s">
+        <v>59</v>
+      </c>
+      <c r="E70">
+        <v>40</v>
+      </c>
+      <c r="F70" t="s">
+        <v>68</v>
+      </c>
+      <c r="G70">
+        <v>4</v>
+      </c>
+      <c r="H70">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" t="s">
+        <v>59</v>
+      </c>
+      <c r="E71">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>68</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73">
+        <v>24</v>
+      </c>
+      <c r="F73" t="s">
+        <v>68</v>
+      </c>
+      <c r="G73">
+        <v>6</v>
+      </c>
+      <c r="H73">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
+        <v>59</v>
+      </c>
+      <c r="E74">
+        <v>35</v>
+      </c>
+      <c r="F74" t="s">
+        <v>68</v>
+      </c>
+      <c r="G74">
+        <v>3.5</v>
+      </c>
+      <c r="H74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>59</v>
+      </c>
+      <c r="E75">
+        <v>40</v>
+      </c>
+      <c r="F75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G75">
+        <v>5</v>
+      </c>
+      <c r="H75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76" t="s">
+        <v>59</v>
+      </c>
+      <c r="E76">
+        <v>30</v>
+      </c>
+      <c r="F76" t="s">
+        <v>68</v>
+      </c>
+      <c r="G76">
+        <v>4.5</v>
+      </c>
+      <c r="H76">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" t="s">
+        <v>59</v>
+      </c>
+      <c r="E77">
+        <v>25</v>
+      </c>
+      <c r="F77" t="s">
+        <v>126</v>
+      </c>
+      <c r="G77">
+        <v>4.5</v>
+      </c>
+      <c r="H77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>59</v>
+      </c>
+      <c r="E78">
+        <v>30</v>
+      </c>
+      <c r="F78" t="s">
+        <v>126</v>
+      </c>
+      <c r="G78">
+        <v>4.5</v>
+      </c>
+      <c r="H78">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79">
+        <v>4.5</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>59</v>
+      </c>
+      <c r="E80">
+        <v>30</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" t="s">
+        <v>20</v>
+      </c>
+      <c r="D81" t="s">
+        <v>59</v>
+      </c>
+      <c r="E81">
+        <v>8</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="H81">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" t="s">
+        <v>59</v>
+      </c>
+      <c r="E82">
+        <v>15</v>
+      </c>
+      <c r="H82">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" t="s">
+        <v>18</v>
+      </c>
+      <c r="D83" t="s">
+        <v>59</v>
+      </c>
+      <c r="E83">
+        <v>30</v>
+      </c>
+      <c r="F83" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83">
+        <v>4</v>
+      </c>
+      <c r="H83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" t="s">
+        <v>59</v>
+      </c>
+      <c r="E84">
+        <v>40</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84">
+        <v>6</v>
+      </c>
+      <c r="H84">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>